<commit_message>
Some fixes: practice questions fixed, saving answers fixed
</commit_message>
<xml_diff>
--- a/data_raw/HPT_dict.xlsx
+++ b/data_raw/HPT_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/HPT_test/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05A956C-6635-4D43-8471-743649EC3100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9992710-187F-4B4B-A7B0-0A8EED798BD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -244,12 +244,6 @@
     <t>Please listen to the following clips and select which chord was different. Select the appropriate number between 1 and 4. These numbers correspond to the order of chords presented.</t>
   </si>
   <si>
-    <t>In diesem Beispiel wurde der zweite Akkord verändert. Die richtige Antwort wäre also Nummer 2. Du kannst gerne noch einmal zuhören, bevor du fortfährst.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Here, the second chord was different, so the correct answer would have been number 2. Feel free to listen again before moving on.</t>
-  </si>
-  <si>
     <t>Zeit zum Üben: \\ **Übungsfrage 1:** \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Akkord verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Akkord gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Akkorde überein.</t>
   </si>
   <si>
@@ -281,6 +275,12 @@
   </si>
   <si>
     <t>Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the different chord. These numbers correspond to the order of chords presented.</t>
+  </si>
+  <si>
+    <t>In diesem Beispiel wurde der dritte Akkord verändert. Die richtige Antwort wäre also **Nummer 3**. Es folgen nun zwei Übungsfragen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Here, the third chord was different, so the correct answer would have been **number 3**. Now you will see two practice questions.</t>
   </si>
 </sst>
 </file>
@@ -697,14 +697,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="75.1640625" customWidth="1"/>
+    <col min="2" max="2" width="126.5" customWidth="1"/>
     <col min="3" max="3" width="101" customWidth="1"/>
   </cols>
   <sheetData>
@@ -925,7 +925,7 @@
         <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -933,10 +933,10 @@
         <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -944,10 +944,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -955,10 +955,10 @@
         <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1007,24 +1007,24 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to style and javascript (play button deleted).
</commit_message>
<xml_diff>
--- a/data_raw/HPT_dict.xlsx
+++ b/data_raw/HPT_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/HPT_test/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9992710-187F-4B4B-A7B0-0A8EED798BD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C843059-5B23-6244-862E-AFF05FCAE5F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,63 +199,27 @@
     <t>SAMPLE1b</t>
   </si>
   <si>
-    <t>Willkommen zum Harmoniefolgen-Unterscheidungstest</t>
-  </si>
-  <si>
     <t>Welcome to the Harmony Progression Discrimination Test</t>
   </si>
   <si>
-    <t>Harmoniefolgen-Unterscheidungstest</t>
-  </si>
-  <si>
-    <t>Du hast den Harmoniefolgen-Unterscheidungstest erfolgreich beendet.</t>
-  </si>
-  <si>
     <t>Harmony Progression Discrimination Test</t>
   </si>
   <si>
     <t>You have completed the Harmony Progression Discrimination Test.</t>
   </si>
   <si>
-    <t>Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Akkord verändert wurde. Wähle die entsprechende Zahl zwischen 1 und 4. Die Zahlen stimmen mit der Reihenfolge der gehörten Akkorde überein.</t>
-  </si>
-  <si>
     <t>With this test we want to investigate how we understand chords. A chord is a group of musical notes played at the same time. \\  For each question on this test, you will hear two short chord progressions consisting of four chords each. The two progressions will be identical with the exception of one chord. Your task is to determine which chord is different by selecting the appropriate number between 1 and 4. These numbers correspond to the order of chords presented.  \\ Please listen to each sound clip in full before making your decision. If you don’t know the answer, give your best guess.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mit diesem Test wollen wir herausfinden, wie unsere Ohren Akkorde wahrnehmen. Ein Akkord ist eine Gruppe von Tönen, die gleichzeitig abgespielt werden. \\ Bei jeder Frage wirst du zwei kurze Akkordfolgen hören, die aus jeweils vier Akkorden bestehen. Die beiden Folgen sind exakt dieselben bis auf einen einzelnen Akkord. Deine Aufgabe ist es herauszufinden, welcher Akkord anders ist, indem du auf die enstrepchende Zahl klickst. Die Zahlen passen zu der Reiehefolge der Akkorde. \\  Bitte höre dir beide Akkordoflgen immer ganz an, bevor du deine Antwort auswählst. Falls du dir nicht sicher bist, wähle einfach deine beste Vermutung aus.  </t>
-  </si>
-  <si>
-    <t>Du hast **{{accuracy}} %** der veränderten Akkorde richtig erkannt.</t>
-  </si>
-  <si>
     <t>You recognized **{{accuracy}} %**  of the altered chords correctly.</t>
   </si>
   <si>
-    <t>Willkommen zur Harmoniefolgen-Unterscheidungsübung. \\ Zuerst wirst du Beispiele hören und dann ein paar Übungsaufgaben machen.</t>
-  </si>
-  <si>
-    <t>Welcome to the Musical Harmony Progression Discrimination Training. \\  Try a couple of practice questions before the test begins.</t>
-  </si>
-  <si>
-    <t>Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Akkord verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Akkord gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Akkorde überein.</t>
-  </si>
-  <si>
     <t>Please listen to the following clips and select which chord was different. Select the appropriate number between 1 and 4. These numbers correspond to the order of chords presented.</t>
   </si>
   <si>
-    <t>Zeit zum Üben: \\ **Übungsfrage 1:** \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Akkord verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Akkord gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Akkorde überein.</t>
-  </si>
-  <si>
-    <t>Time for some practice: \\ **Practice question 1:** \\ Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the differenct chord. These numbers correspond to the order of chords presented.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> **{{feedback}}** \\ Here’s another example. \\ **Practice question 2:** \\ Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the differenct chord. These numbers correspond to the order of chords presented.</t>
   </si>
   <si>
-    <t>**{{feedback}}** \\ Hier ist ein weiteres Beispiel. \\ **Übungsfrage 2:** \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Akkord verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Akkord gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Akkorde überein.</t>
-  </si>
-  <si>
     <t>RESULTS_SAVED</t>
   </si>
   <si>
@@ -274,13 +238,49 @@
     <t>Du kannst den Browsertab jetzt schließen.</t>
   </si>
   <si>
-    <t>Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the different chord. These numbers correspond to the order of chords presented.</t>
-  </si>
-  <si>
-    <t>In diesem Beispiel wurde der dritte Akkord verändert. Die richtige Antwort wäre also **Nummer 3**. Es folgen nun zwei Übungsfragen.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Here, the third chord was different, so the correct answer would have been **number 3**. Now you will see two practice questions.</t>
+  </si>
+  <si>
+    <t>Zuerst wirst du Beispiele hören und dann ein paar Übungsaufgaben machen.</t>
+  </si>
+  <si>
+    <t>Try a couple of practice questions before the test begins.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit diesem Test wollen wir herausfinden, wie unsere Ohren Dreiklänge wahrnehmen. Ein Dreiklang ist eine Gruppe von drei Tönen, die gleichzeitig abgespielt werden. \\ Bei jeder Frage wirst du zwei kurze Dreiklangsfolgen hören, die aus jeweils vier Dreiklängen bestehen. Die beiden Folgen sind exakt dieselben bis auf einen einzelnen Dreiklang. Deine Aufgabe ist es herauszufinden, welcher Dreiklang anders ist, indem du auf die entsprechende Zahl klickst. Die Zahlen passen zu der Reihenfolge der Dreiklänge. \\  Bitte höre dir beide Dreiklangsfolgen immer ganz an, bevor du deine Antwort auswählst. Falls du dir nicht sicher bist, wähle einfach deine beste Vermutung aus.  </t>
+  </si>
+  <si>
+    <t>Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Dreiklang verändert wurde. Wähle die entsprechende Zahl zwischen 1 und 4. Die Zahlen stimmen mit der Reihenfolge der gehörten Dreiklänge überein.</t>
+  </si>
+  <si>
+    <t>Du hast **{{accuracy}} %** der veränderten Dreiklänge richtig erkannt.</t>
+  </si>
+  <si>
+    <t>In diesem Beispiel wurde der dritte Dreiklang verändert. Die richtige Antwort wäre also **Nummer 3**. Es folgen nun zwei Übungsfragen.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Hier ist ein weiteres Beispiel. \\ **Übungsfrage 2:** \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Dreiklang verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Dreiklang gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Dreiklänge überein.</t>
+  </si>
+  <si>
+    <t>Willkommen zum Dreiklangsfolgen-Test</t>
+  </si>
+  <si>
+    <t>Du hast den Dreiklangsfolgen-Test erfolgreich beendet.</t>
+  </si>
+  <si>
+    <t>Dreiklangsfolgen-Test</t>
+  </si>
+  <si>
+    <t>Zuerst wirst du Beispiele hören und dann ein paar Übungsaufgaben machen. \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Dreikläng verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Dreiklänge gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Dreiklänge überein.</t>
+  </si>
+  <si>
+    <t>Try a couple of practice questions before the test begins. \\ Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the different chord. These numbers correspond to the order of chords presented.</t>
+  </si>
+  <si>
+    <t>**Übungsfrage 1** \\ Bitte höre dir die folgenden Musikausschnitte an und entscheide, welcher Dreiklang verändert wurde. Überlege dir welche Zahle zwischen 1 und 4 zu dem veränderten Dreiklänge gehört. Die Zahlen stimmen mit der Reihenfolge der gehörten Dreiklänge überein.</t>
+  </si>
+  <si>
+    <t>**Practice question 1** \\ Please listen to the following clips and select which chord was different. Think about which number between 1 and 4 fits the differenct chord. These numbers correspond to the order of chords presented.</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -724,10 +724,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -735,10 +735,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -768,10 +768,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -801,10 +801,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -845,10 +845,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -856,10 +856,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -911,10 +911,10 @@
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -922,7 +922,7 @@
         <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>84</v>
@@ -933,10 +933,10 @@
         <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -944,10 +944,10 @@
         <v>46</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -955,10 +955,10 @@
         <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1007,24 +1007,24 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>